<commit_message>
Criação de pasta para artefatos do Estudo Orientado
</commit_message>
<xml_diff>
--- a/Avaliação/Performance.xlsx
+++ b/Avaliação/Performance.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Lista de repositórios obtida em https://git.wiki.kernel.org/index.php/GitProjects</t>
   </si>
@@ -140,6 +140,15 @@
   </si>
   <si>
     <t>Size (MB)</t>
+  </si>
+  <si>
+    <t>Insert 1st</t>
+  </si>
+  <si>
+    <t>Insert 2nd</t>
+  </si>
+  <si>
+    <t>N/D</t>
   </si>
 </sst>
 </file>
@@ -171,7 +180,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,6 +190,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -213,13 +228,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -525,23 +541,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="61.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -554,8 +570,10 @@
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -566,10 +584,11 @@
         <v>23</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
       <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -589,390 +608,506 @@
         <v>19</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>1</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="C4" s="1">
-        <v>23922</v>
+        <v>187</v>
       </c>
       <c r="D4" s="1">
-        <v>84.4</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <f>9290</f>
-        <v>9290</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
+        <v>539</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6</v>
+      </c>
+      <c r="G4" s="1">
+        <v>12.4</v>
+      </c>
+      <c r="H4" s="1">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1.7</v>
+      </c>
+      <c r="J4" s="1">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K4" s="1">
+        <v>3.5</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C5" s="1">
-        <v>184</v>
+        <v>443</v>
       </c>
       <c r="D5" s="1">
-        <v>1</v>
+        <v>3.4</v>
       </c>
       <c r="E5" s="1">
-        <v>539</v>
-      </c>
-      <c r="F5" s="1">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2.7</v>
-      </c>
-      <c r="H5" s="1">
-        <v>6.4</v>
-      </c>
-      <c r="I5" s="1">
-        <v>3.5</v>
-      </c>
-      <c r="J5" s="1">
-        <v>2.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>815</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1">
-        <v>3775</v>
+        <v>535</v>
       </c>
       <c r="D6" s="1">
-        <v>27</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E6" s="1">
-        <v>1478</v>
+        <v>502</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="1">
+        <v>702</v>
+      </c>
+      <c r="D7" s="1">
         <v>7</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1">
-        <v>25822</v>
-      </c>
-      <c r="D7" s="1">
-        <v>141</v>
-      </c>
       <c r="E7" s="1">
-        <v>20729</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>685</v>
+      </c>
+      <c r="F7" s="1">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>20.8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>22.6</v>
+      </c>
+      <c r="I7" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="J7" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="K7" s="1">
+        <v>5.6</v>
+      </c>
+      <c r="L7" s="1">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1">
-        <v>35260</v>
+        <v>2979</v>
       </c>
       <c r="D8" s="1">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
-        <v>2656</v>
-      </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1595</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>42.4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>46</v>
+      </c>
+      <c r="I8" s="1">
+        <v>5.9</v>
+      </c>
+      <c r="J8" s="1">
+        <v>6.8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="L8" s="1">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3775</v>
+      </c>
+      <c r="D9" s="1">
         <v>27</v>
       </c>
-      <c r="C9" s="1">
-        <v>6417</v>
-      </c>
-      <c r="D9" s="1">
-        <v>448</v>
-      </c>
       <c r="E9" s="1">
-        <v>1549</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1478</v>
+      </c>
+      <c r="F9" s="1">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1">
+        <v>49.6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>46.6</v>
+      </c>
+      <c r="I9" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>7.3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>3.7</v>
+      </c>
+      <c r="L9" s="1">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
-        <v>535</v>
+        <v>5518</v>
       </c>
       <c r="D10" s="1">
-        <v>4.5999999999999996</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1">
-        <v>502</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>253</v>
+      </c>
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>40</v>
+      </c>
+      <c r="H10" s="1">
+        <v>37.4</v>
+      </c>
+      <c r="I10" s="1">
+        <v>1.4</v>
+      </c>
+      <c r="J10" s="1">
+        <v>9.4</v>
+      </c>
+      <c r="K10" s="1">
+        <v>65</v>
+      </c>
+      <c r="L10" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1">
-        <v>2979</v>
+        <v>6166</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>85</v>
       </c>
       <c r="E11" s="1">
-        <v>1595</v>
+        <v>3220</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1">
-        <v>5518</v>
+        <v>6417</v>
       </c>
       <c r="D12" s="1">
-        <v>20</v>
+        <v>448</v>
       </c>
       <c r="E12" s="1">
-        <v>253</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>35</v>
+        <v>1549</v>
+      </c>
+      <c r="F12" s="1">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>155.80000000000001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>129</v>
+      </c>
+      <c r="I12" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="J12" s="1">
+        <v>10.6</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L12" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="1">
-        <v>443</v>
+        <v>23922</v>
       </c>
       <c r="D13" s="1">
-        <v>3.4</v>
+        <v>84.4</v>
       </c>
       <c r="E13" s="1">
-        <v>815</v>
+        <f>9290</f>
+        <v>9290</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>7</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
-        <v>427109</v>
+        <v>25822</v>
       </c>
       <c r="D14" s="1">
-        <v>818</v>
+        <v>141</v>
       </c>
       <c r="E14" s="1">
-        <f>45948</f>
-        <v>45948</v>
+        <v>20729</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="1">
+        <v>35260</v>
+      </c>
+      <c r="D15" s="1">
+        <v>98</v>
+      </c>
+      <c r="E15" s="1">
+        <v>2656</v>
+      </c>
+      <c r="F15" s="1">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1">
+        <v>196</v>
+      </c>
+      <c r="H15" s="1">
+        <v>158.6</v>
+      </c>
+      <c r="I15" s="1">
+        <v>3.4</v>
+      </c>
+      <c r="J15" s="1">
+        <v>40</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L15" s="1">
+        <v>19.399999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B16" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="1">
         <v>42434</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D16" s="1">
         <v>117</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E16" s="1">
         <v>2777</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="1">
-        <v>702</v>
-      </c>
-      <c r="D16" s="1">
-        <v>7</v>
-      </c>
-      <c r="E16" s="1">
-        <v>685</v>
-      </c>
-      <c r="F16" s="1">
-        <v>11</v>
-      </c>
-      <c r="G16" s="1">
-        <v>3.6</v>
-      </c>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
       <c r="H16" s="1"/>
-      <c r="I16" s="1">
-        <v>5.6</v>
-      </c>
-      <c r="J16" s="1">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>13</v>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
-        <v>6166</v>
+        <v>56326</v>
       </c>
       <c r="D17" s="1">
-        <v>85</v>
+        <v>261</v>
       </c>
       <c r="E17" s="1">
-        <v>3220</v>
+        <v>10393</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>14</v>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>12</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1">
-        <v>56326</v>
+        <v>427109</v>
       </c>
       <c r="D18" s="1">
-        <v>261</v>
+        <v>818</v>
       </c>
       <c r="E18" s="1">
-        <v>10393</v>
+        <f>45948</f>
+        <v>45948</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H21" s="4"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J21" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A4:J18">
-    <sortCondition ref="A4:A18"/>
+  <sortState ref="A4:L18">
+    <sortCondition ref="C4:C18"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B7" r:id="rId2"/>
-    <hyperlink ref="B9" r:id="rId3"/>
-    <hyperlink ref="B10" r:id="rId4"/>
-    <hyperlink ref="B11" r:id="rId5"/>
-    <hyperlink ref="B12" r:id="rId6"/>
-    <hyperlink ref="B17" r:id="rId7"/>
-    <hyperlink ref="B18" r:id="rId8"/>
-    <hyperlink ref="B5" r:id="rId9"/>
-    <hyperlink ref="B13" r:id="rId10"/>
-    <hyperlink ref="B16" r:id="rId11"/>
-    <hyperlink ref="B8" r:id="rId12"/>
-    <hyperlink ref="B14" r:id="rId13"/>
-    <hyperlink ref="B15" r:id="rId14"/>
+    <hyperlink ref="B9" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId2"/>
+    <hyperlink ref="B12" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId4"/>
+    <hyperlink ref="B8" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B11" r:id="rId7"/>
+    <hyperlink ref="B17" r:id="rId8"/>
+    <hyperlink ref="B4" r:id="rId9"/>
+    <hyperlink ref="B5" r:id="rId10"/>
+    <hyperlink ref="B7" r:id="rId11"/>
+    <hyperlink ref="B15" r:id="rId12"/>
+    <hyperlink ref="B18" r:id="rId13"/>
+    <hyperlink ref="B16" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>

</xml_diff>

<commit_message>
Working on comments made to the paper.
</commit_message>
<xml_diff>
--- a/Avaliação/Performance.xlsx
+++ b/Avaliação/Performance.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="48">
   <si>
     <t>Lista de repositórios obtida em https://git.wiki.kernel.org/index.php/GitProjects</t>
   </si>
@@ -153,6 +153,15 @@
   <si>
     <t>Project</t>
   </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Operation</t>
+  </si>
+  <si>
+    <t># nodes</t>
+  </si>
 </sst>
 </file>
 
@@ -218,7 +227,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -250,12 +259,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -281,6 +299,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -946,7 +967,7 @@
                   <c:v>18.399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.7</c:v>
+                  <c:v>21.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>65</c:v>
@@ -1052,7 +1073,7 @@
                   <c:v>3.4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.3</c:v>
+                  <c:v>3.7</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4.0999999999999996</c:v>
@@ -1085,11 +1106,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218992528"/>
-        <c:axId val="218998800"/>
+        <c:axId val="299894784"/>
+        <c:axId val="299893216"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218992528"/>
+        <c:axId val="299894784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1202,12 +1223,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218998800"/>
+        <c:crossAx val="299893216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218998800"/>
+        <c:axId val="299893216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1320,7 +1341,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218992528"/>
+        <c:crossAx val="299894784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1416,7 +1437,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2156,11 +2176,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218992920"/>
-        <c:axId val="218994488"/>
+        <c:axId val="14164832"/>
+        <c:axId val="14163656"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218992920"/>
+        <c:axId val="14164832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2181,7 +2201,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2248,12 +2267,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218994488"/>
+        <c:crossAx val="14163656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218994488"/>
+        <c:axId val="14163656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2274,7 +2293,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2341,7 +2359,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218992920"/>
+        <c:crossAx val="14164832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2355,7 +2373,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2437,7 +2454,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3177,11 +3193,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218389008"/>
-        <c:axId val="218389400"/>
+        <c:axId val="14164440"/>
+        <c:axId val="14162088"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218389008"/>
+        <c:axId val="14164440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3202,7 +3218,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3269,12 +3284,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218389400"/>
+        <c:crossAx val="14162088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218389400"/>
+        <c:axId val="14162088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3295,7 +3310,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3362,7 +3376,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218389008"/>
+        <c:crossAx val="14164440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3376,7 +3390,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4197,11 +4210,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="218390968"/>
-        <c:axId val="218391752"/>
+        <c:axId val="14166792"/>
+        <c:axId val="14159344"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="218390968"/>
+        <c:axId val="14166792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4288,12 +4301,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218391752"/>
+        <c:crossAx val="14159344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="218391752"/>
+        <c:axId val="14159344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4380,7 +4393,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="218390968"/>
+        <c:crossAx val="14166792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7117,10 +7130,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7136,9 +7149,11 @@
     <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7154,7 +7169,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -7170,7 +7185,7 @@
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>44</v>
       </c>
@@ -7207,8 +7222,23 @@
       <c r="L3" s="13" t="s">
         <v>17</v>
       </c>
+      <c r="N3" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" s="16" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -7245,8 +7275,27 @@
       <c r="L4" s="8">
         <v>2.7</v>
       </c>
+      <c r="N4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O4">
+        <f>PEARSON(C$4:C$13,$G$4:$G$13)</f>
+        <v>0.79496056142586968</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:R4" si="0">PEARSON(D$4:D$13,$G$4:$G$13)</f>
+        <v>0.65261806406866363</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>0.30070908363860865</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>-0.44444773139753008</v>
+      </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -7283,8 +7332,27 @@
       <c r="L5" s="8">
         <v>3.2</v>
       </c>
+      <c r="N5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5">
+        <f>PEARSON(C$4:C$13,$H$4:$H$13)</f>
+        <v>0.81549683918223947</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ref="P5:R5" si="1">PEARSON(D$4:D$13,$H$4:$H$13)</f>
+        <v>0.64529556444529634</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>0.3626698136877885</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="1"/>
+        <v>-0.46281831793086081</v>
+      </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -7321,8 +7389,27 @@
       <c r="L6" s="8">
         <v>3.4</v>
       </c>
+      <c r="N6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6">
+        <f>PEARSON(C$4:C$13,$I$4:$I$13)</f>
+        <v>1.2274770639508343E-3</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ref="P6:R6" si="2">PEARSON(D$4:D$13,$I$4:$I$13)</f>
+        <v>-0.28302669106362144</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="2"/>
+        <v>-0.13048180107333365</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="2"/>
+        <v>-0.25396479215497747</v>
+      </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -7354,13 +7441,32 @@
         <v>7.3</v>
       </c>
       <c r="K7" s="8">
+        <v>21.3</v>
+      </c>
+      <c r="L7" s="8">
         <v>3.7</v>
       </c>
-      <c r="L7" s="8">
-        <v>21.3</v>
+      <c r="N7" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="O7">
+        <f>PEARSON(C$4:C$13,$J$4:$J$13)</f>
+        <v>0.94014128674106023</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ref="P7:R7" si="3">PEARSON(D$4:D$13,$J$4:$J$13)</f>
+        <v>0.16980203580720488</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>0.3300902280638498</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>-0.35485415778579443</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
@@ -7397,8 +7503,27 @@
       <c r="L8" s="8">
         <v>4.0999999999999996</v>
       </c>
+      <c r="N8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="O8">
+        <f>PEARSON(C$4:C$9,$K$4:$K$9)</f>
+        <v>0.94050951845206565</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:R8" si="4">PEARSON(D$4:D$9,$K$4:$K$9)</f>
+        <v>0.74886529465122764</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="4"/>
+        <v>0.42530465742076989</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>-0.59182581659085742</v>
+      </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -7435,8 +7560,27 @@
       <c r="L9" s="8">
         <v>4.2</v>
       </c>
+      <c r="N9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9">
+        <f>PEARSON(C$4:C$13,$L$4:$L$13)</f>
+        <v>0.86113486403720185</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:R9" si="5">PEARSON(D$4:D$13,$L$4:$L$13)</f>
+        <v>0.60885496758138757</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="5"/>
+        <v>0.5923971065066137</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="5"/>
+        <v>-0.39252513710021819</v>
+      </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -7472,7 +7616,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
@@ -7509,7 +7653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -7545,7 +7689,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -7581,7 +7725,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -7595,7 +7739,7 @@
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>16</v>
       </c>
@@ -7618,8 +7762,9 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
       <c r="L15" s="8"/>
+      <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Updates to paper (v3)
</commit_message>
<xml_diff>
--- a/Avaliação/Performance.xlsx
+++ b/Avaliação/Performance.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="74">
   <si>
     <t>Lista de repositórios obtida em https://git.wiki.kernel.org/index.php/GitProjects</t>
   </si>
@@ -160,7 +160,85 @@
     <t>Operation</t>
   </si>
   <si>
-    <t># nodes</t>
+    <t># peers</t>
+  </si>
+  <si>
+    <t>Pearson</t>
+  </si>
+  <si>
+    <t>Commits rank</t>
+  </si>
+  <si>
+    <t>Size rank</t>
+  </si>
+  <si>
+    <t>Files rank</t>
+  </si>
+  <si>
+    <t>peers rank</t>
+  </si>
+  <si>
+    <t>insert 1st rank</t>
+  </si>
+  <si>
+    <t>insert 2nd rank</t>
+  </si>
+  <si>
+    <t>check branches rank</t>
+  </si>
+  <si>
+    <t>update topology rank</t>
+  </si>
+  <si>
+    <t>commit history rank</t>
+  </si>
+  <si>
+    <t>topology rank</t>
+  </si>
+  <si>
+    <t>Spearman</t>
+  </si>
+  <si>
+    <t>Metrics ranks</t>
+  </si>
+  <si>
+    <t>Diff^2 commits</t>
+  </si>
+  <si>
+    <t>Diff^2 size</t>
+  </si>
+  <si>
+    <t>Diff^2 files</t>
+  </si>
+  <si>
+    <t>Diff^2 peers</t>
+  </si>
+  <si>
+    <t>Update topology</t>
+  </si>
+  <si>
+    <t>soma</t>
+  </si>
+  <si>
+    <t>6*soma</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>n(n^2-1)</t>
+  </si>
+  <si>
+    <t>1-(num/den)</t>
+  </si>
+  <si>
+    <t>Memory (MB)</t>
+  </si>
+  <si>
+    <t>Memory footprint</t>
+  </si>
+  <si>
+    <t>Memory Commit History</t>
   </si>
 </sst>
 </file>
@@ -273,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -297,11 +375,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -975,6 +1054,9 @@
                 <c:pt idx="5">
                   <c:v>68</c:v>
                 </c:pt>
+                <c:pt idx="6">
+                  <c:v>73</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -985,7 +1067,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Dados por Commit'!$L$3</c:f>
+              <c:f>'Dados por Commit'!$O$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1059,7 +1141,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Dados por Commit'!$L$4:$L$13</c:f>
+              <c:f>'Dados por Commit'!$O$4:$O$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1106,11 +1188,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="299894784"/>
-        <c:axId val="299893216"/>
+        <c:axId val="262854984"/>
+        <c:axId val="262855376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="299894784"/>
+        <c:axId val="262854984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1223,12 +1305,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299893216"/>
+        <c:crossAx val="262855376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="299893216"/>
+        <c:axId val="262855376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,7 +1423,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="299894784"/>
+        <c:crossAx val="262854984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1437,6 +1519,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2176,11 +2259,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="14164832"/>
-        <c:axId val="14163656"/>
+        <c:axId val="262854200"/>
+        <c:axId val="262853024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14164832"/>
+        <c:axId val="262854200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2201,6 +2284,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2267,12 +2351,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14163656"/>
+        <c:crossAx val="262853024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14163656"/>
+        <c:axId val="262853024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2293,6 +2377,7 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2359,7 +2444,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14164832"/>
+        <c:crossAx val="262854200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2373,6 +2458,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3193,11 +3279,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="14164440"/>
-        <c:axId val="14162088"/>
+        <c:axId val="262852632"/>
+        <c:axId val="262858904"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14164440"/>
+        <c:axId val="262852632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3284,12 +3370,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14162088"/>
+        <c:crossAx val="262858904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14162088"/>
+        <c:axId val="262858904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3376,7 +3462,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14164440"/>
+        <c:crossAx val="262852632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4210,11 +4296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="14166792"/>
-        <c:axId val="14159344"/>
+        <c:axId val="262859296"/>
+        <c:axId val="262858120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="14166792"/>
+        <c:axId val="262859296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4301,12 +4387,12 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14159344"/>
+        <c:crossAx val="262858120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="14159344"/>
+        <c:axId val="262858120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4393,7 +4479,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14166792"/>
+        <c:crossAx val="262859296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6702,15 +6788,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>590551</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7130,10 +7216,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R22"/>
+  <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="AZ8" sqref="AZ8:BC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7148,12 +7234,33 @@
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="8" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
-    <col min="14" max="14" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="7.28515625" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" customWidth="1"/>
+    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="16" max="16" width="9" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="6" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="6.5703125" hidden="1" customWidth="1"/>
+    <col min="20" max="24" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="9" hidden="1" customWidth="1"/>
+    <col min="26" max="29" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="8" hidden="1" customWidth="1"/>
+    <col min="31" max="34" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="8" hidden="1" customWidth="1"/>
+    <col min="36" max="39" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="7.28515625" hidden="1" customWidth="1"/>
+    <col min="41" max="44" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="45" max="45" width="8" hidden="1" customWidth="1"/>
+    <col min="46" max="49" width="8.42578125" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="8.85546875" customWidth="1"/>
+    <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7168,24 +7275,115 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+      <c r="Z1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
+      <c r="AJ1" s="1"/>
+      <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
+      <c r="AM1" s="1"/>
+      <c r="AN1" s="1"/>
+      <c r="AO1" s="1"/>
+      <c r="AP1" s="1"/>
+      <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
+      <c r="AW1" s="1"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17"/>
+      <c r="T2" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="17"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="17"/>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17"/>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17"/>
+      <c r="AL2" s="17"/>
+      <c r="AM2" s="17"/>
+      <c r="AN2" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17"/>
+      <c r="AQ2" s="17"/>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="AT2" s="17"/>
+      <c r="AU2" s="17"/>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="17"/>
+      <c r="AZ2" t="s">
+        <v>48</v>
+      </c>
     </row>
-    <row r="3" spans="1:18" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" ht="51" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>44</v>
       </c>
@@ -7202,7 +7400,7 @@
         <v>37</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>18</v>
+        <v>47</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>39</v>
@@ -7219,26 +7417,137 @@
       <c r="K3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="P3" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q3" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T3" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="V3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="W3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AB3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AD3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="AE3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AF3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AG3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AI3" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AK3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="AO3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AP3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AQ3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AR3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AS3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="AT3" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV3" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="O3" s="16" t="s">
+      <c r="AZ3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="BA3" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="Q3" s="16" t="s">
+      <c r="BB3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="R3" s="16" t="s">
+      <c r="BC3" s="15" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -7273,29 +7582,161 @@
         <v>3.5</v>
       </c>
       <c r="L4" s="8">
+        <v>61</v>
+      </c>
+      <c r="M4" s="8">
+        <v>76</v>
+      </c>
+      <c r="N4" s="8">
+        <f>M4-L4</f>
+        <v>15</v>
+      </c>
+      <c r="O4" s="8">
         <v>2.7</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="P4" s="8">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>10</v>
+      </c>
+      <c r="R4" s="8">
+        <v>9</v>
+      </c>
+      <c r="S4" s="8">
+        <v>2</v>
+      </c>
+      <c r="T4" s="8">
+        <v>10</v>
+      </c>
+      <c r="U4" s="8">
+        <f>(P4-$T4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="8">
+        <f t="shared" ref="V4:X13" si="0">(Q4-$T4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="W4" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X4" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="8">
+        <f>(P4-$Y4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="8">
+        <f t="shared" ref="AA4:AC13" si="1">(Q4-$Y4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC4" s="8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="AD4" s="8">
+        <v>7</v>
+      </c>
+      <c r="AE4" s="8">
+        <f>(P4-$AD4)^2</f>
+        <v>9</v>
+      </c>
+      <c r="AF4" s="8">
+        <f t="shared" ref="AF4:AH13" si="2">(Q4-$AD4)^2</f>
+        <v>9</v>
+      </c>
+      <c r="AG4" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AH4" s="8">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AI4" s="8">
+        <v>10</v>
+      </c>
+      <c r="AJ4" s="8">
+        <f>(P4-$AI4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AK4" s="8">
+        <f t="shared" ref="AK4:AM13" si="3">(Q4-$AI4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AL4" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM4" s="8">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="AN4" s="8">
+        <v>6</v>
+      </c>
+      <c r="AO4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="8">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="8">
+        <v>16</v>
+      </c>
+      <c r="AS4" s="8">
+        <v>10</v>
+      </c>
+      <c r="AT4" s="8">
+        <f>(P4-$AS4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AU4" s="8">
+        <f t="shared" ref="AU4:AW13" si="4">(Q4-$AS4)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AV4" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AW4" s="8">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="AY4" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="O4">
+      <c r="AZ4" s="16">
         <f>PEARSON(C$4:C$13,$G$4:$G$13)</f>
         <v>0.79496056142586968</v>
       </c>
-      <c r="P4">
-        <f t="shared" ref="P4:R4" si="0">PEARSON(D$4:D$13,$G$4:$G$13)</f>
+      <c r="BA4" s="16">
+        <f>PEARSON(D$4:D$13,$G$4:$G$13)</f>
         <v>0.65261806406866363</v>
       </c>
-      <c r="Q4">
-        <f t="shared" si="0"/>
+      <c r="BB4" s="16">
+        <f>PEARSON(E$4:E$13,$G$4:$G$13)</f>
         <v>0.30070908363860865</v>
       </c>
-      <c r="R4">
-        <f t="shared" si="0"/>
+      <c r="BC4" s="16">
+        <f>PEARSON(F$4:F$13,$G$4:$G$13)</f>
         <v>-0.44444773139753008</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -7330,29 +7771,161 @@
         <v>5.6</v>
       </c>
       <c r="L5" s="8">
+        <v>69</v>
+      </c>
+      <c r="M5" s="8">
+        <v>88</v>
+      </c>
+      <c r="N5" s="8">
+        <f t="shared" ref="N5:N13" si="5">M5-L5</f>
+        <v>19</v>
+      </c>
+      <c r="O5" s="8">
         <v>3.2</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="P5" s="8">
+        <v>9</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>9</v>
+      </c>
+      <c r="R5" s="8">
+        <v>8</v>
+      </c>
+      <c r="S5" s="8">
+        <v>1</v>
+      </c>
+      <c r="T5" s="8">
+        <v>9</v>
+      </c>
+      <c r="U5" s="8">
+        <f t="shared" ref="U5:U13" si="6">(P5-$T5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="V5" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W5" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X5" s="8">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>9</v>
+      </c>
+      <c r="Z5" s="8">
+        <f t="shared" ref="Z5:Z13" si="7">(P5-$Y5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AA5" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB5" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC5" s="8">
+        <f t="shared" si="1"/>
+        <v>64</v>
+      </c>
+      <c r="AD5" s="8">
+        <v>6</v>
+      </c>
+      <c r="AE5" s="8">
+        <f t="shared" ref="AE5:AE13" si="8">(P5-$AD5)^2</f>
+        <v>9</v>
+      </c>
+      <c r="AF5" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AG5" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AH5" s="8">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AI5" s="8">
+        <v>9</v>
+      </c>
+      <c r="AJ5" s="8">
+        <f t="shared" ref="AJ5:AJ13" si="9">(P5-$AI5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AK5" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AL5" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM5" s="8">
+        <f t="shared" si="3"/>
+        <v>64</v>
+      </c>
+      <c r="AN5" s="8">
+        <v>5</v>
+      </c>
+      <c r="AO5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="8">
+        <v>1</v>
+      </c>
+      <c r="AR5" s="8">
+        <v>16</v>
+      </c>
+      <c r="AS5" s="8">
+        <v>9</v>
+      </c>
+      <c r="AT5" s="8">
+        <f t="shared" ref="AT5:AT13" si="10">(P5-$AS5)^2</f>
+        <v>0</v>
+      </c>
+      <c r="AU5" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV5" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AW5" s="8">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="AY5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O5">
+      <c r="AZ5" s="16">
         <f>PEARSON(C$4:C$13,$H$4:$H$13)</f>
         <v>0.81549683918223947</v>
       </c>
-      <c r="P5">
-        <f t="shared" ref="P5:R5" si="1">PEARSON(D$4:D$13,$H$4:$H$13)</f>
+      <c r="BA5" s="16">
+        <f>PEARSON(D$4:D$13,$H$4:$H$13)</f>
         <v>0.64529556444529634</v>
       </c>
-      <c r="Q5">
-        <f t="shared" si="1"/>
+      <c r="BB5" s="16">
+        <f>PEARSON(E$4:E$13,$H$4:$H$13)</f>
         <v>0.3626698136877885</v>
       </c>
-      <c r="R5">
-        <f t="shared" si="1"/>
+      <c r="BC5" s="16">
+        <f>PEARSON(F$4:F$13,$H$4:$H$13)</f>
         <v>-0.46281831793086081</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -7387,29 +7960,161 @@
         <v>18.399999999999999</v>
       </c>
       <c r="L6" s="8">
+        <v>118</v>
+      </c>
+      <c r="M6" s="8">
+        <v>630</v>
+      </c>
+      <c r="N6" s="8">
+        <f t="shared" si="5"/>
+        <v>512</v>
+      </c>
+      <c r="O6" s="8">
         <v>3.4</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="P6" s="8">
+        <v>8</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>8</v>
+      </c>
+      <c r="R6" s="8">
+        <v>5</v>
+      </c>
+      <c r="S6" s="8">
+        <v>7</v>
+      </c>
+      <c r="T6" s="8">
+        <v>6</v>
+      </c>
+      <c r="U6" s="8">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="V6" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W6" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="X6" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Y6" s="8">
+        <v>6</v>
+      </c>
+      <c r="Z6" s="8">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AA6" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AB6" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AC6" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AD6" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="8">
+        <f t="shared" si="8"/>
+        <v>49</v>
+      </c>
+      <c r="AF6" s="8">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="AG6" s="8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="AH6" s="8">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="AI6" s="8">
+        <v>8</v>
+      </c>
+      <c r="AJ6" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK6" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AL6" s="8">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="AM6" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AN6" s="8">
+        <v>4</v>
+      </c>
+      <c r="AO6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="8">
+        <v>9</v>
+      </c>
+      <c r="AR6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="8">
+        <v>8</v>
+      </c>
+      <c r="AT6" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU6" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV6" s="8">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AW6" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AY6" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="O6">
+      <c r="AZ6" s="16">
         <f>PEARSON(C$4:C$13,$I$4:$I$13)</f>
         <v>1.2274770639508343E-3</v>
       </c>
-      <c r="P6">
-        <f t="shared" ref="P6:R6" si="2">PEARSON(D$4:D$13,$I$4:$I$13)</f>
+      <c r="BA6" s="16">
+        <f>PEARSON(D$4:D$13,$I$4:$I$13)</f>
         <v>-0.28302669106362144</v>
       </c>
-      <c r="Q6">
-        <f t="shared" si="2"/>
+      <c r="BB6" s="16">
+        <f>PEARSON(E$4:E$13,$I$4:$I$13)</f>
         <v>-0.13048180107333365</v>
       </c>
-      <c r="R6">
-        <f t="shared" si="2"/>
+      <c r="BC6" s="16">
+        <f>PEARSON(F$4:F$13,$I$4:$I$13)</f>
         <v>-0.25396479215497747</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>6</v>
       </c>
@@ -7444,29 +8149,161 @@
         <v>21.3</v>
       </c>
       <c r="L7" s="8">
+        <v>127</v>
+      </c>
+      <c r="M7" s="8">
+        <v>686</v>
+      </c>
+      <c r="N7" s="8">
+        <f t="shared" si="5"/>
+        <v>559</v>
+      </c>
+      <c r="O7" s="8">
         <v>3.7</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="P7" s="8">
+        <v>7</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>6</v>
+      </c>
+      <c r="R7" s="8">
+        <v>7</v>
+      </c>
+      <c r="S7" s="8">
+        <v>9</v>
+      </c>
+      <c r="T7" s="8">
+        <v>5</v>
+      </c>
+      <c r="U7" s="8">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="V7" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W7" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X7" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="Y7" s="8">
+        <v>5</v>
+      </c>
+      <c r="Z7" s="8">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AA7" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB7" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AC7" s="8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AD7" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE7" s="8">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="AF7" s="8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="AG7" s="8">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AH7" s="8">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="AI7" s="8">
+        <v>7</v>
+      </c>
+      <c r="AJ7" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK7" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AL7" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AM7" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AN7" s="8">
+        <v>3</v>
+      </c>
+      <c r="AO7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="8">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="8">
+        <v>4</v>
+      </c>
+      <c r="AS7" s="8">
+        <v>7</v>
+      </c>
+      <c r="AT7" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU7" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AV7" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AW7" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AY7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="O7">
+      <c r="AZ7" s="16">
         <f>PEARSON(C$4:C$13,$J$4:$J$13)</f>
         <v>0.94014128674106023</v>
       </c>
-      <c r="P7">
-        <f t="shared" ref="P7:R7" si="3">PEARSON(D$4:D$13,$J$4:$J$13)</f>
+      <c r="BA7" s="16">
+        <f>PEARSON(D$4:D$13,$J$4:$J$13)</f>
         <v>0.16980203580720488</v>
       </c>
-      <c r="Q7">
-        <f t="shared" si="3"/>
+      <c r="BB7" s="16">
+        <f>PEARSON(E$4:E$13,$J$4:$J$13)</f>
         <v>0.3300902280638498</v>
       </c>
-      <c r="R7">
-        <f t="shared" si="3"/>
+      <c r="BC7" s="16">
+        <f>PEARSON(F$4:F$13,$J$4:$J$13)</f>
         <v>-0.35485415778579443</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
@@ -7501,29 +8338,161 @@
         <v>65</v>
       </c>
       <c r="L8" s="8">
+        <v>134</v>
+      </c>
+      <c r="M8" s="8">
+        <v>1255</v>
+      </c>
+      <c r="N8" s="8">
+        <f t="shared" si="5"/>
+        <v>1121</v>
+      </c>
+      <c r="O8" s="8">
         <v>4.0999999999999996</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="P8" s="8">
+        <v>6</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>7</v>
+      </c>
+      <c r="R8" s="8">
+        <v>10</v>
+      </c>
+      <c r="S8" s="8">
+        <v>10</v>
+      </c>
+      <c r="T8" s="8">
+        <v>7</v>
+      </c>
+      <c r="U8" s="8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V8" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W8" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="X8" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Y8" s="8">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AA8" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB8" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AC8" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AD8" s="8">
+        <v>10</v>
+      </c>
+      <c r="AE8" s="8">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="AF8" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AG8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AI8" s="8">
+        <v>6</v>
+      </c>
+      <c r="AJ8" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK8" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AL8" s="8">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="AM8" s="8">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="AN8" s="8">
+        <v>2</v>
+      </c>
+      <c r="AO8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="8">
+        <v>1</v>
+      </c>
+      <c r="AQ8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="8">
+        <v>16</v>
+      </c>
+      <c r="AS8" s="8">
+        <v>6</v>
+      </c>
+      <c r="AT8" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU8" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AV8" s="8">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="AW8" s="8">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="AY8" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="O8">
-        <f>PEARSON(C$4:C$9,$K$4:$K$9)</f>
-        <v>0.94050951845206565</v>
-      </c>
-      <c r="P8">
-        <f t="shared" ref="P8:R8" si="4">PEARSON(D$4:D$9,$K$4:$K$9)</f>
-        <v>0.74886529465122764</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="4"/>
-        <v>0.42530465742076989</v>
-      </c>
-      <c r="R8">
-        <f t="shared" si="4"/>
-        <v>-0.59182581659085742</v>
+      <c r="AZ8" s="16">
+        <f>PEARSON(C$4:C$10,$K$4:$K$10)</f>
+        <v>0.9539806087578675</v>
+      </c>
+      <c r="BA8" s="16">
+        <f t="shared" ref="BA8:BC8" si="11">PEARSON(D$4:D$10,$K$4:$K$10)</f>
+        <v>0.62469516499133659</v>
+      </c>
+      <c r="BB8" s="16">
+        <f t="shared" si="11"/>
+        <v>0.41156623238126616</v>
+      </c>
+      <c r="BC8" s="16">
+        <f t="shared" si="11"/>
+        <v>-0.61029282800962048</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
@@ -7558,29 +8527,161 @@
         <v>68</v>
       </c>
       <c r="L9" s="8">
+        <v>183</v>
+      </c>
+      <c r="M9" s="8">
+        <v>675</v>
+      </c>
+      <c r="N9" s="8">
+        <f t="shared" si="5"/>
+        <v>492</v>
+      </c>
+      <c r="O9" s="8">
         <v>4.2</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="P9" s="8">
+        <v>5</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>4</v>
+      </c>
+      <c r="R9" s="8">
+        <v>3</v>
+      </c>
+      <c r="S9" s="8">
+        <v>5</v>
+      </c>
+      <c r="T9" s="8">
+        <v>8</v>
+      </c>
+      <c r="U9" s="8">
+        <f t="shared" si="6"/>
+        <v>9</v>
+      </c>
+      <c r="V9" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="W9" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="X9" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Y9" s="8">
+        <v>8</v>
+      </c>
+      <c r="Z9" s="8">
+        <f t="shared" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="AA9" s="8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AB9" s="8">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="AC9" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AD9" s="8">
+        <v>9</v>
+      </c>
+      <c r="AE9" s="8">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="AF9" s="8">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="AG9" s="8">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="AH9" s="8">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="AI9" s="8">
+        <v>5</v>
+      </c>
+      <c r="AJ9" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK9" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AL9" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AM9" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AN9" s="8">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="8">
+        <v>4</v>
+      </c>
+      <c r="AR9" s="8">
+        <v>4</v>
+      </c>
+      <c r="AS9" s="8">
+        <v>5</v>
+      </c>
+      <c r="AT9" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU9" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AV9" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AW9" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AY9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="O9">
-        <f>PEARSON(C$4:C$13,$L$4:$L$13)</f>
+      <c r="AZ9" s="16">
+        <f>PEARSON(C$4:C$13,$O$4:$O$13)</f>
         <v>0.86113486403720185</v>
       </c>
-      <c r="P9">
-        <f t="shared" ref="P9:R9" si="5">PEARSON(D$4:D$13,$L$4:$L$13)</f>
+      <c r="BA9" s="16">
+        <f>PEARSON(D$4:D$13,$O$4:$O$13)</f>
         <v>0.60885496758138757</v>
       </c>
-      <c r="Q9">
-        <f t="shared" si="5"/>
+      <c r="BB9" s="16">
+        <f>PEARSON(E$4:E$13,$O$4:$O$13)</f>
         <v>0.5923971065066137</v>
       </c>
-      <c r="R9">
-        <f t="shared" si="5"/>
+      <c r="BC9" s="16">
+        <f>PEARSON(F$4:F$13,$O$4:$O$13)</f>
         <v>-0.39252513710021819</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
@@ -7611,12 +8712,136 @@
       <c r="J10" s="8">
         <v>10.6</v>
       </c>
-      <c r="K10" s="8"/>
+      <c r="K10" s="8">
+        <v>73</v>
+      </c>
       <c r="L10" s="8">
+        <v>138</v>
+      </c>
+      <c r="M10" s="8">
+        <v>1667</v>
+      </c>
+      <c r="N10" s="8">
+        <f t="shared" si="5"/>
+        <v>1529</v>
+      </c>
+      <c r="O10" s="8">
         <v>17</v>
       </c>
+      <c r="P10" s="8">
+        <v>4</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>1</v>
+      </c>
+      <c r="R10" s="8">
+        <v>6</v>
+      </c>
+      <c r="S10" s="8">
+        <v>8</v>
+      </c>
+      <c r="T10" s="8">
+        <v>2</v>
+      </c>
+      <c r="U10" s="8">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="V10" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W10" s="8">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="X10" s="8">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="Y10" s="8">
+        <v>2</v>
+      </c>
+      <c r="Z10" s="8">
+        <f t="shared" si="7"/>
+        <v>4</v>
+      </c>
+      <c r="AA10" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB10" s="8">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="AC10" s="8">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="AD10" s="8">
+        <v>8</v>
+      </c>
+      <c r="AE10" s="8">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="AF10" s="8">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="AG10" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AH10" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AI10" s="8">
+        <v>4</v>
+      </c>
+      <c r="AJ10" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK10" s="8">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="AL10" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AM10" s="8">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="AN10" s="8"/>
+      <c r="AO10" s="8"/>
+      <c r="AP10" s="8"/>
+      <c r="AQ10" s="8"/>
+      <c r="AR10" s="8"/>
+      <c r="AS10" s="8">
+        <v>4</v>
+      </c>
+      <c r="AT10" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU10" s="8">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AV10" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AW10" s="8">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>5</v>
       </c>
@@ -7649,11 +8874,132 @@
         <v>18</v>
       </c>
       <c r="K11" s="8"/>
-      <c r="L11" s="8">
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O11" s="8">
         <v>18</v>
       </c>
+      <c r="P11" s="8">
+        <v>3</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>5</v>
+      </c>
+      <c r="R11" s="8">
+        <v>2</v>
+      </c>
+      <c r="S11" s="8">
+        <v>4</v>
+      </c>
+      <c r="T11" s="8">
+        <v>4</v>
+      </c>
+      <c r="U11" s="8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V11" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W11" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y11" s="8">
+        <v>4</v>
+      </c>
+      <c r="Z11" s="8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AA11" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB11" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AC11" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD11" s="8">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AF11" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG11" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AH11" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AI11" s="8">
+        <v>3</v>
+      </c>
+      <c r="AJ11" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK11" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AL11" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM11" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AN11" s="8"/>
+      <c r="AO11" s="8"/>
+      <c r="AP11" s="8"/>
+      <c r="AQ11" s="8"/>
+      <c r="AR11" s="8"/>
+      <c r="AS11" s="8">
+        <v>3</v>
+      </c>
+      <c r="AT11" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU11" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AV11" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AW11" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AZ11" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
@@ -7685,11 +9031,129 @@
         <v>19.3</v>
       </c>
       <c r="K12" s="8"/>
-      <c r="L12" s="8">
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O12" s="8">
         <v>18.2</v>
       </c>
+      <c r="P12" s="8">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>2</v>
+      </c>
+      <c r="R12" s="8">
+        <v>1</v>
+      </c>
+      <c r="S12" s="8">
+        <v>3</v>
+      </c>
+      <c r="T12" s="8">
+        <v>3</v>
+      </c>
+      <c r="U12" s="8">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="V12" s="8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="W12" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="X12" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y12" s="8">
+        <v>3</v>
+      </c>
+      <c r="Z12" s="8">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="AA12" s="8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AB12" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AC12" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD12" s="8">
+        <v>4</v>
+      </c>
+      <c r="AE12" s="8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AF12" s="8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="AG12" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AH12" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AI12" s="8">
+        <v>2</v>
+      </c>
+      <c r="AJ12" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK12" s="8">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AL12" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AM12" s="8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AN12" s="8"/>
+      <c r="AO12" s="8"/>
+      <c r="AP12" s="8"/>
+      <c r="AQ12" s="8"/>
+      <c r="AR12" s="8"/>
+      <c r="AS12" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT12" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU12" s="8">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AV12" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AW12" s="8">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>15</v>
       </c>
@@ -7721,11 +9185,144 @@
         <v>40</v>
       </c>
       <c r="K13" s="8"/>
-      <c r="L13" s="8">
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
         <v>19.399999999999999</v>
       </c>
+      <c r="P13" s="8">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>3</v>
+      </c>
+      <c r="R13" s="8">
+        <v>4</v>
+      </c>
+      <c r="S13" s="8">
+        <v>6</v>
+      </c>
+      <c r="T13" s="8">
+        <v>1</v>
+      </c>
+      <c r="U13" s="8">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="8">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="W13" s="8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="X13" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="Y13" s="8">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="8">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="AB13" s="8">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="AC13" s="8">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>3</v>
+      </c>
+      <c r="AE13" s="8">
+        <f t="shared" si="8"/>
+        <v>4</v>
+      </c>
+      <c r="AF13" s="8">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AG13" s="8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AH13" s="8">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="AI13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="8">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AK13" s="8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="AL13" s="8">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="AM13" s="8">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="AN13" s="8"/>
+      <c r="AO13" s="8"/>
+      <c r="AP13" s="8"/>
+      <c r="AQ13" s="8"/>
+      <c r="AR13" s="8"/>
+      <c r="AS13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AT13" s="8">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="AU13" s="8">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AV13" s="8">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AW13" s="8">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="AY13" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="AZ13" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="BA13" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="BB13" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC13" s="15" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="14" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
@@ -7738,154 +9335,1203 @@
       <c r="J14" s="11"/>
       <c r="K14" s="11"/>
       <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="U14" s="11">
+        <f>SUM(U4:U13)</f>
+        <v>24</v>
+      </c>
+      <c r="V14" s="11">
+        <f t="shared" ref="V14:X14" si="12">SUM(V4:V13)</f>
+        <v>28</v>
+      </c>
+      <c r="W14" s="11">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="X14" s="11">
+        <f t="shared" si="12"/>
+        <v>224</v>
+      </c>
+      <c r="Y14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z14" s="11">
+        <f>SUM(Z4:Z13)</f>
+        <v>24</v>
+      </c>
+      <c r="AA14" s="11">
+        <f t="shared" ref="AA14" si="13">SUM(AA4:AA13)</f>
+        <v>28</v>
+      </c>
+      <c r="AB14" s="11">
+        <f t="shared" ref="AB14" si="14">SUM(AB4:AB13)</f>
+        <v>74</v>
+      </c>
+      <c r="AC14" s="11">
+        <f t="shared" ref="AC14" si="15">SUM(AC4:AC13)</f>
+        <v>224</v>
+      </c>
+      <c r="AD14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AE14" s="11">
+        <f>SUM(AE4:AE13)</f>
+        <v>152</v>
+      </c>
+      <c r="AF14" s="11">
+        <f t="shared" ref="AF14" si="16">SUM(AF4:AF13)</f>
+        <v>170</v>
+      </c>
+      <c r="AG14" s="11">
+        <f t="shared" ref="AG14" si="17">SUM(AG4:AG13)</f>
+        <v>108</v>
+      </c>
+      <c r="AH14" s="11">
+        <f t="shared" ref="AH14" si="18">SUM(AH4:AH13)</f>
+        <v>162</v>
+      </c>
+      <c r="AI14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ14" s="11">
+        <f>SUM(AJ4:AJ13)</f>
+        <v>0</v>
+      </c>
+      <c r="AK14" s="11">
+        <f t="shared" ref="AK14" si="19">SUM(AK4:AK13)</f>
+        <v>20</v>
+      </c>
+      <c r="AL14" s="11">
+        <f t="shared" ref="AL14" si="20">SUM(AL4:AL13)</f>
+        <v>46</v>
+      </c>
+      <c r="AM14" s="11">
+        <f t="shared" ref="AM14" si="21">SUM(AM4:AM13)</f>
+        <v>192</v>
+      </c>
+      <c r="AN14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AO14" s="11">
+        <f>SUM(AO4:AO13)</f>
+        <v>0</v>
+      </c>
+      <c r="AP14" s="11">
+        <f t="shared" ref="AP14" si="22">SUM(AP4:AP13)</f>
+        <v>2</v>
+      </c>
+      <c r="AQ14" s="11">
+        <f t="shared" ref="AQ14" si="23">SUM(AQ4:AQ13)</f>
+        <v>15</v>
+      </c>
+      <c r="AR14" s="11">
+        <f t="shared" ref="AR14" si="24">SUM(AR4:AR13)</f>
+        <v>56</v>
+      </c>
+      <c r="AS14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AT14" s="11">
+        <f>SUM(AT4:AT13)</f>
+        <v>0</v>
+      </c>
+      <c r="AU14" s="11">
+        <f t="shared" ref="AU14" si="25">SUM(AU4:AU13)</f>
+        <v>20</v>
+      </c>
+      <c r="AV14" s="11">
+        <f t="shared" ref="AV14" si="26">SUM(AV4:AV13)</f>
+        <v>46</v>
+      </c>
+      <c r="AW14" s="11">
+        <f t="shared" ref="AW14" si="27">SUM(AW4:AW13)</f>
+        <v>192</v>
+      </c>
+      <c r="AY14" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="AZ14" s="16">
+        <f>U18</f>
+        <v>0.8545454545454545</v>
+      </c>
+      <c r="BA14" s="16">
+        <f t="shared" ref="BA14:BC14" si="28">V18</f>
+        <v>0.83030303030303032</v>
+      </c>
+      <c r="BB14" s="16">
+        <f t="shared" si="28"/>
+        <v>0.55151515151515151</v>
+      </c>
+      <c r="BC14" s="16">
+        <f t="shared" si="28"/>
+        <v>-0.35757575757575766</v>
+      </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="U15" s="11">
+        <f>6*U14</f>
+        <v>144</v>
+      </c>
+      <c r="V15" s="11">
+        <f t="shared" ref="V15:X15" si="29">6*V14</f>
+        <v>168</v>
+      </c>
+      <c r="W15" s="11">
+        <f t="shared" si="29"/>
+        <v>444</v>
+      </c>
+      <c r="X15" s="11">
+        <f t="shared" si="29"/>
+        <v>1344</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z15" s="11">
+        <f>6*Z14</f>
+        <v>144</v>
+      </c>
+      <c r="AA15" s="11">
+        <f t="shared" ref="AA15" si="30">6*AA14</f>
+        <v>168</v>
+      </c>
+      <c r="AB15" s="11">
+        <f t="shared" ref="AB15" si="31">6*AB14</f>
+        <v>444</v>
+      </c>
+      <c r="AC15" s="11">
+        <f t="shared" ref="AC15" si="32">6*AC14</f>
+        <v>1344</v>
+      </c>
+      <c r="AD15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE15" s="11">
+        <f>6*AE14</f>
+        <v>912</v>
+      </c>
+      <c r="AF15" s="11">
+        <f t="shared" ref="AF15" si="33">6*AF14</f>
+        <v>1020</v>
+      </c>
+      <c r="AG15" s="11">
+        <f t="shared" ref="AG15" si="34">6*AG14</f>
+        <v>648</v>
+      </c>
+      <c r="AH15" s="11">
+        <f t="shared" ref="AH15" si="35">6*AH14</f>
+        <v>972</v>
+      </c>
+      <c r="AI15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AJ15" s="11">
+        <f>6*AJ14</f>
+        <v>0</v>
+      </c>
+      <c r="AK15" s="11">
+        <f t="shared" ref="AK15" si="36">6*AK14</f>
+        <v>120</v>
+      </c>
+      <c r="AL15" s="11">
+        <f t="shared" ref="AL15" si="37">6*AL14</f>
+        <v>276</v>
+      </c>
+      <c r="AM15" s="11">
+        <f t="shared" ref="AM15" si="38">6*AM14</f>
+        <v>1152</v>
+      </c>
+      <c r="AN15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AO15" s="11">
+        <f>6*AO14</f>
+        <v>0</v>
+      </c>
+      <c r="AP15" s="11">
+        <f t="shared" ref="AP15" si="39">6*AP14</f>
+        <v>12</v>
+      </c>
+      <c r="AQ15" s="11">
+        <f t="shared" ref="AQ15" si="40">6*AQ14</f>
+        <v>90</v>
+      </c>
+      <c r="AR15" s="11">
+        <f t="shared" ref="AR15" si="41">6*AR14</f>
+        <v>336</v>
+      </c>
+      <c r="AS15" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="AT15" s="11">
+        <f>6*AT14</f>
+        <v>0</v>
+      </c>
+      <c r="AU15" s="11">
+        <f t="shared" ref="AU15" si="42">6*AU14</f>
+        <v>120</v>
+      </c>
+      <c r="AV15" s="11">
+        <f t="shared" ref="AV15" si="43">6*AV14</f>
+        <v>276</v>
+      </c>
+      <c r="AW15" s="11">
+        <f t="shared" ref="AW15" si="44">6*AW14</f>
+        <v>1152</v>
+      </c>
+      <c r="AY15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="AZ15" s="16">
+        <f>Z18</f>
+        <v>0.8545454545454545</v>
+      </c>
+      <c r="BA15" s="16">
+        <f t="shared" ref="BA15:BC15" si="45">AA18</f>
+        <v>0.83030303030303032</v>
+      </c>
+      <c r="BB15" s="16">
+        <f t="shared" si="45"/>
+        <v>0.55151515151515151</v>
+      </c>
+      <c r="BC15" s="16">
+        <f t="shared" si="45"/>
+        <v>-0.35757575757575766</v>
+      </c>
+    </row>
+    <row r="16" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="U16" s="11">
+        <f>COUNT(U4:U13)</f>
+        <v>10</v>
+      </c>
+      <c r="V16" s="11">
+        <f t="shared" ref="V16:X16" si="46">COUNT(V4:V13)</f>
+        <v>10</v>
+      </c>
+      <c r="W16" s="11">
+        <f t="shared" si="46"/>
+        <v>10</v>
+      </c>
+      <c r="X16" s="11">
+        <f t="shared" si="46"/>
+        <v>10</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z16" s="11">
+        <f>COUNT(Z4:Z13)</f>
+        <v>10</v>
+      </c>
+      <c r="AA16" s="11">
+        <f t="shared" ref="AA16:AC16" si="47">COUNT(AA4:AA13)</f>
+        <v>10</v>
+      </c>
+      <c r="AB16" s="11">
+        <f t="shared" si="47"/>
+        <v>10</v>
+      </c>
+      <c r="AC16" s="11">
+        <f t="shared" si="47"/>
+        <v>10</v>
+      </c>
+      <c r="AD16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE16" s="11">
+        <f>COUNT(AE4:AE13)</f>
+        <v>10</v>
+      </c>
+      <c r="AF16" s="11">
+        <f t="shared" ref="AF16:AH16" si="48">COUNT(AF4:AF13)</f>
+        <v>10</v>
+      </c>
+      <c r="AG16" s="11">
+        <f t="shared" si="48"/>
+        <v>10</v>
+      </c>
+      <c r="AH16" s="11">
+        <f t="shared" si="48"/>
+        <v>10</v>
+      </c>
+      <c r="AI16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AJ16" s="11">
+        <f>COUNT(AJ4:AJ13)</f>
+        <v>10</v>
+      </c>
+      <c r="AK16" s="11">
+        <f t="shared" ref="AK16:AM16" si="49">COUNT(AK4:AK13)</f>
+        <v>10</v>
+      </c>
+      <c r="AL16" s="11">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+      <c r="AM16" s="11">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+      <c r="AN16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AO16" s="11">
+        <f>COUNT(AO4:AO13)</f>
+        <v>6</v>
+      </c>
+      <c r="AP16" s="11">
+        <f t="shared" ref="AP16:AR16" si="50">COUNT(AP4:AP13)</f>
+        <v>6</v>
+      </c>
+      <c r="AQ16" s="11">
+        <f t="shared" si="50"/>
+        <v>6</v>
+      </c>
+      <c r="AR16" s="11">
+        <f t="shared" si="50"/>
+        <v>6</v>
+      </c>
+      <c r="AS16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT16" s="11">
+        <f>COUNT(AT4:AT13)</f>
+        <v>10</v>
+      </c>
+      <c r="AU16" s="11">
+        <f t="shared" ref="AU16:AW16" si="51">COUNT(AU4:AU13)</f>
+        <v>10</v>
+      </c>
+      <c r="AV16" s="11">
+        <f t="shared" si="51"/>
+        <v>10</v>
+      </c>
+      <c r="AW16" s="11">
+        <f t="shared" si="51"/>
+        <v>10</v>
+      </c>
+      <c r="AY16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AZ16" s="16">
+        <f>AE18</f>
+        <v>7.878787878787874E-2</v>
+      </c>
+      <c r="BA16" s="16">
+        <f t="shared" ref="BA16:BC16" si="52">AF18</f>
+        <v>-3.0303030303030276E-2</v>
+      </c>
+      <c r="BB16" s="16">
+        <f t="shared" si="52"/>
+        <v>0.34545454545454546</v>
+      </c>
+      <c r="BC16" s="16">
+        <f t="shared" si="52"/>
+        <v>1.8181818181818188E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="U17" s="11">
+        <f>U16*(U16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="V17" s="11">
+        <f t="shared" ref="V17:X17" si="53">V16*(V16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="W17" s="11">
+        <f t="shared" si="53"/>
+        <v>990</v>
+      </c>
+      <c r="X17" s="11">
+        <f t="shared" si="53"/>
+        <v>990</v>
+      </c>
+      <c r="Y17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z17" s="11">
+        <f>Z16*(Z16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AA17" s="11">
+        <f t="shared" ref="AA17" si="54">AA16*(AA16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AB17" s="11">
+        <f t="shared" ref="AB17" si="55">AB16*(AB16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AC17" s="11">
+        <f t="shared" ref="AC17" si="56">AC16*(AC16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AD17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE17" s="11">
+        <f>AE16*(AE16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AF17" s="11">
+        <f t="shared" ref="AF17" si="57">AF16*(AF16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AG17" s="11">
+        <f t="shared" ref="AG17" si="58">AG16*(AG16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AH17" s="11">
+        <f t="shared" ref="AH17" si="59">AH16*(AH16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AI17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AJ17" s="11">
+        <f>AJ16*(AJ16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AK17" s="11">
+        <f t="shared" ref="AK17" si="60">AK16*(AK16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AL17" s="11">
+        <f t="shared" ref="AL17" si="61">AL16*(AL16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AM17" s="11">
+        <f t="shared" ref="AM17" si="62">AM16*(AM16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AN17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO17" s="11">
+        <f>AO16*(AO16^2-1)</f>
+        <v>210</v>
+      </c>
+      <c r="AP17" s="11">
+        <f t="shared" ref="AP17" si="63">AP16*(AP16^2-1)</f>
+        <v>210</v>
+      </c>
+      <c r="AQ17" s="11">
+        <f t="shared" ref="AQ17" si="64">AQ16*(AQ16^2-1)</f>
+        <v>210</v>
+      </c>
+      <c r="AR17" s="11">
+        <f t="shared" ref="AR17" si="65">AR16*(AR16^2-1)</f>
+        <v>210</v>
+      </c>
+      <c r="AS17" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="AT17" s="11">
+        <f>AT16*(AT16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AU17" s="11">
+        <f t="shared" ref="AU17" si="66">AU16*(AU16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AV17" s="11">
+        <f t="shared" ref="AV17" si="67">AV16*(AV16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AW17" s="11">
+        <f t="shared" ref="AW17" si="68">AW16*(AW16^2-1)</f>
+        <v>990</v>
+      </c>
+      <c r="AY17" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="AZ17" s="16">
+        <f>AJ18</f>
+        <v>1</v>
+      </c>
+      <c r="BA17" s="16">
+        <f t="shared" ref="BA17:BC17" si="69">AK18</f>
+        <v>0.87878787878787878</v>
+      </c>
+      <c r="BB17" s="16">
+        <f t="shared" si="69"/>
+        <v>0.72121212121212119</v>
+      </c>
+      <c r="BC17" s="16">
+        <f t="shared" si="69"/>
+        <v>-0.16363636363636358</v>
+      </c>
+    </row>
+    <row r="18" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="U18" s="11">
+        <f>1-(U15/U17)</f>
+        <v>0.8545454545454545</v>
+      </c>
+      <c r="V18" s="11">
+        <f t="shared" ref="V18:X18" si="70">1-(V15/V17)</f>
+        <v>0.83030303030303032</v>
+      </c>
+      <c r="W18" s="11">
+        <f t="shared" si="70"/>
+        <v>0.55151515151515151</v>
+      </c>
+      <c r="X18" s="11">
+        <f t="shared" si="70"/>
+        <v>-0.35757575757575766</v>
+      </c>
+      <c r="Y18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z18" s="11">
+        <f>1-(Z15/Z17)</f>
+        <v>0.8545454545454545</v>
+      </c>
+      <c r="AA18" s="11">
+        <f t="shared" ref="AA18" si="71">1-(AA15/AA17)</f>
+        <v>0.83030303030303032</v>
+      </c>
+      <c r="AB18" s="11">
+        <f t="shared" ref="AB18" si="72">1-(AB15/AB17)</f>
+        <v>0.55151515151515151</v>
+      </c>
+      <c r="AC18" s="11">
+        <f t="shared" ref="AC18" si="73">1-(AC15/AC17)</f>
+        <v>-0.35757575757575766</v>
+      </c>
+      <c r="AD18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE18" s="11">
+        <f>1-(AE15/AE17)</f>
+        <v>7.878787878787874E-2</v>
+      </c>
+      <c r="AF18" s="11">
+        <f t="shared" ref="AF18" si="74">1-(AF15/AF17)</f>
+        <v>-3.0303030303030276E-2</v>
+      </c>
+      <c r="AG18" s="11">
+        <f t="shared" ref="AG18" si="75">1-(AG15/AG17)</f>
+        <v>0.34545454545454546</v>
+      </c>
+      <c r="AH18" s="11">
+        <f t="shared" ref="AH18" si="76">1-(AH15/AH17)</f>
+        <v>1.8181818181818188E-2</v>
+      </c>
+      <c r="AI18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AJ18" s="11">
+        <f>1-(AJ15/AJ17)</f>
+        <v>1</v>
+      </c>
+      <c r="AK18" s="11">
+        <f t="shared" ref="AK18" si="77">1-(AK15/AK17)</f>
+        <v>0.87878787878787878</v>
+      </c>
+      <c r="AL18" s="11">
+        <f t="shared" ref="AL18" si="78">1-(AL15/AL17)</f>
+        <v>0.72121212121212119</v>
+      </c>
+      <c r="AM18" s="11">
+        <f t="shared" ref="AM18" si="79">1-(AM15/AM17)</f>
+        <v>-0.16363636363636358</v>
+      </c>
+      <c r="AN18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO18" s="11">
+        <f>1-(AO15/AO17)</f>
+        <v>1</v>
+      </c>
+      <c r="AP18" s="11">
+        <f t="shared" ref="AP18" si="80">1-(AP15/AP17)</f>
+        <v>0.94285714285714284</v>
+      </c>
+      <c r="AQ18" s="11">
+        <f t="shared" ref="AQ18" si="81">1-(AQ15/AQ17)</f>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="AR18" s="11">
+        <f t="shared" ref="AR18" si="82">1-(AR15/AR17)</f>
+        <v>-0.60000000000000009</v>
+      </c>
+      <c r="AS18" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="AT18" s="11">
+        <f>1-(AT15/AT17)</f>
+        <v>1</v>
+      </c>
+      <c r="AU18" s="11">
+        <f t="shared" ref="AU18" si="83">1-(AU15/AU17)</f>
+        <v>0.87878787878787878</v>
+      </c>
+      <c r="AV18" s="11">
+        <f t="shared" ref="AV18" si="84">1-(AV15/AV17)</f>
+        <v>0.72121212121212119</v>
+      </c>
+      <c r="AW18" s="11">
+        <f t="shared" ref="AW18" si="85">1-(AW15/AW17)</f>
+        <v>-0.16363636363636358</v>
+      </c>
+      <c r="AY18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ18" s="16">
+        <f>AO18</f>
+        <v>1</v>
+      </c>
+      <c r="BA18" s="16">
+        <f t="shared" ref="BA18:BC18" si="86">AP18</f>
+        <v>0.94285714285714284</v>
+      </c>
+      <c r="BB18" s="16">
+        <f t="shared" si="86"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="BC18" s="16">
+        <f t="shared" si="86"/>
+        <v>-0.60000000000000009</v>
+      </c>
+    </row>
+    <row r="19" spans="1:55" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
+      <c r="U19" s="11"/>
+      <c r="V19" s="11"/>
+      <c r="W19" s="11"/>
+      <c r="X19" s="11"/>
+      <c r="Y19" s="11"/>
+      <c r="Z19" s="11"/>
+      <c r="AA19" s="11"/>
+      <c r="AB19" s="11"/>
+      <c r="AC19" s="11"/>
+      <c r="AD19" s="11"/>
+      <c r="AE19" s="11"/>
+      <c r="AF19" s="11"/>
+      <c r="AG19" s="11"/>
+      <c r="AH19" s="11"/>
+      <c r="AI19" s="11"/>
+      <c r="AJ19" s="11"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="11"/>
+      <c r="AM19" s="11"/>
+      <c r="AN19" s="11"/>
+      <c r="AO19" s="11"/>
+      <c r="AP19" s="11"/>
+      <c r="AQ19" s="11"/>
+      <c r="AR19" s="11"/>
+      <c r="AS19" s="11"/>
+      <c r="AT19" s="11"/>
+      <c r="AU19" s="11"/>
+      <c r="AV19" s="11"/>
+      <c r="AW19" s="11"/>
+      <c r="AY19" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AZ19" s="16">
+        <f>AT18</f>
+        <v>1</v>
+      </c>
+      <c r="BA19" s="16">
+        <f t="shared" ref="BA19:BC19" si="87">AU18</f>
+        <v>0.87878787878787878</v>
+      </c>
+      <c r="BB19" s="16">
+        <f t="shared" si="87"/>
+        <v>0.72121212121212119</v>
+      </c>
+      <c r="BC19" s="16">
+        <f t="shared" si="87"/>
+        <v>-0.16363636363636358</v>
+      </c>
+    </row>
+    <row r="20" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B20" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C20" s="8">
         <v>443</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D20" s="8">
         <v>3.4</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E20" s="8">
         <v>815</v>
       </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="O15" s="3"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8"/>
+      <c r="M20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="P20" s="8">
+        <v>443</v>
+      </c>
+      <c r="Q20" s="8">
+        <v>3.4</v>
+      </c>
+      <c r="R20" s="8">
+        <v>815</v>
+      </c>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="8"/>
+      <c r="Y20" s="8"/>
+      <c r="Z20" s="8"/>
+      <c r="AA20" s="8"/>
+      <c r="AB20" s="8"/>
+      <c r="AC20" s="8"/>
+      <c r="AD20" s="8"/>
+      <c r="AE20" s="8"/>
+      <c r="AF20" s="8"/>
+      <c r="AG20" s="8"/>
+      <c r="AH20" s="8"/>
+      <c r="AI20" s="8"/>
+      <c r="AJ20" s="8"/>
+      <c r="AK20" s="8"/>
+      <c r="AL20" s="8"/>
+      <c r="AM20" s="8"/>
+      <c r="AN20" s="8"/>
+      <c r="AO20" s="8"/>
+      <c r="AP20" s="8"/>
+      <c r="AQ20" s="8"/>
+      <c r="AR20" s="8"/>
+      <c r="AS20" s="8"/>
+      <c r="AT20" s="8"/>
+      <c r="AU20" s="8"/>
+      <c r="AV20" s="8"/>
+      <c r="AW20" s="8"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+    <row r="21" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A21" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C21" s="8">
         <v>535</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D21" s="8">
         <v>4.5999999999999996</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E21" s="8">
         <v>502</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8">
+        <v>535</v>
+      </c>
+      <c r="Q21" s="8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R21" s="8">
+        <v>502</v>
+      </c>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="U21" s="8"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+      <c r="AN21" s="8"/>
+      <c r="AO21" s="8"/>
+      <c r="AP21" s="8"/>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="8"/>
+      <c r="AS21" s="8"/>
+      <c r="AT21" s="8"/>
+      <c r="AU21" s="8"/>
+      <c r="AV21" s="8"/>
+      <c r="AW21" s="8"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="12" t="s">
+    <row r="22" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A22" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C22" s="8">
         <v>42434</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D22" s="8">
         <v>117</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E22" s="8">
         <v>2777</v>
       </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8"/>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8"/>
+      <c r="P22" s="8">
+        <v>42434</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>117</v>
+      </c>
+      <c r="R22" s="8">
+        <v>2777</v>
+      </c>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="U22" s="8"/>
+      <c r="V22" s="8"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="8"/>
+      <c r="Y22" s="8"/>
+      <c r="Z22" s="8"/>
+      <c r="AA22" s="8"/>
+      <c r="AB22" s="8"/>
+      <c r="AC22" s="8"/>
+      <c r="AD22" s="8"/>
+      <c r="AE22" s="8"/>
+      <c r="AF22" s="8"/>
+      <c r="AG22" s="8"/>
+      <c r="AH22" s="8"/>
+      <c r="AI22" s="8"/>
+      <c r="AJ22" s="8"/>
+      <c r="AK22" s="8"/>
+      <c r="AL22" s="8"/>
+      <c r="AM22" s="8"/>
+      <c r="AN22" s="8"/>
+      <c r="AO22" s="8"/>
+      <c r="AP22" s="8"/>
+      <c r="AQ22" s="8"/>
+      <c r="AR22" s="8"/>
+      <c r="AS22" s="8"/>
+      <c r="AT22" s="8"/>
+      <c r="AU22" s="8"/>
+      <c r="AV22" s="8"/>
+      <c r="AW22" s="8"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+    <row r="23" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B23" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C23" s="8">
         <v>56326</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D23" s="8">
         <v>261</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E23" s="8">
         <v>10393</v>
       </c>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="8"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="8">
+        <v>56326</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>261</v>
+      </c>
+      <c r="R23" s="8">
+        <v>10393</v>
+      </c>
+      <c r="S23" s="8"/>
+      <c r="T23" s="8"/>
+      <c r="U23" s="8"/>
+      <c r="V23" s="8"/>
+      <c r="W23" s="8"/>
+      <c r="X23" s="8"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
+      <c r="AC23" s="8"/>
+      <c r="AD23" s="8"/>
+      <c r="AE23" s="8"/>
+      <c r="AF23" s="8"/>
+      <c r="AG23" s="8"/>
+      <c r="AH23" s="8"/>
+      <c r="AI23" s="8"/>
+      <c r="AJ23" s="8"/>
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="8"/>
+      <c r="AN23" s="8"/>
+      <c r="AO23" s="8"/>
+      <c r="AP23" s="8"/>
+      <c r="AQ23" s="8"/>
+      <c r="AR23" s="8"/>
+      <c r="AS23" s="8"/>
+      <c r="AT23" s="8"/>
+      <c r="AU23" s="8"/>
+      <c r="AV23" s="8"/>
+      <c r="AW23" s="8"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
+    <row r="24" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A24" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B24" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C24" s="8">
         <v>427109</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D24" s="8">
         <v>818</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E24" s="8">
         <f>45948</f>
         <v>45948</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="8"/>
+      <c r="M24" s="8"/>
+      <c r="N24" s="8"/>
+      <c r="O24" s="8"/>
+      <c r="P24" s="8">
+        <v>427109</v>
+      </c>
+      <c r="Q24" s="8">
+        <v>818</v>
+      </c>
+      <c r="R24" s="8">
+        <f>45948</f>
+        <v>45948</v>
+      </c>
+      <c r="S24" s="8"/>
+      <c r="T24" s="8"/>
+      <c r="U24" s="8"/>
+      <c r="V24" s="8"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="8"/>
+      <c r="Y24" s="8"/>
+      <c r="Z24" s="8"/>
+      <c r="AA24" s="8"/>
+      <c r="AB24" s="8"/>
+      <c r="AC24" s="8"/>
+      <c r="AD24" s="8"/>
+      <c r="AE24" s="8"/>
+      <c r="AF24" s="8"/>
+      <c r="AG24" s="8"/>
+      <c r="AH24" s="8"/>
+      <c r="AI24" s="8"/>
+      <c r="AJ24" s="8"/>
+      <c r="AK24" s="8"/>
+      <c r="AL24" s="8"/>
+      <c r="AM24" s="8"/>
+      <c r="AN24" s="8"/>
+      <c r="AO24" s="8"/>
+      <c r="AP24" s="8"/>
+      <c r="AQ24" s="8"/>
+      <c r="AR24" s="8"/>
+      <c r="AS24" s="8"/>
+      <c r="AT24" s="8"/>
+      <c r="AU24" s="8"/>
+      <c r="AV24" s="8"/>
+      <c r="AW24" s="8"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J22" s="2"/>
+    <row r="27" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="J27" s="2"/>
+      <c r="AI27" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A4:L18">
-    <sortCondition ref="C4:C18"/>
+  <sortState ref="C4:V13">
+    <sortCondition ref="C4:C13"/>
   </sortState>
-  <mergeCells count="1">
-    <mergeCell ref="G2:I2"/>
+  <mergeCells count="8">
+    <mergeCell ref="G2:O2"/>
+    <mergeCell ref="AD2:AH2"/>
+    <mergeCell ref="AI2:AM2"/>
+    <mergeCell ref="AN2:AR2"/>
+    <mergeCell ref="AS2:AW2"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="T2:X2"/>
+    <mergeCell ref="Y2:AC2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1"/>
     <hyperlink ref="B12" r:id="rId2"/>
     <hyperlink ref="B10" r:id="rId3"/>
-    <hyperlink ref="B16" r:id="rId4"/>
+    <hyperlink ref="B21" r:id="rId4"/>
     <hyperlink ref="B6" r:id="rId5"/>
     <hyperlink ref="B8" r:id="rId6"/>
     <hyperlink ref="B9" r:id="rId7"/>
-    <hyperlink ref="B18" r:id="rId8"/>
+    <hyperlink ref="B23" r:id="rId8"/>
     <hyperlink ref="B4" r:id="rId9"/>
-    <hyperlink ref="B15" r:id="rId10"/>
+    <hyperlink ref="B20" r:id="rId10"/>
     <hyperlink ref="B5" r:id="rId11"/>
     <hyperlink ref="B13" r:id="rId12"/>
-    <hyperlink ref="B19" r:id="rId13"/>
-    <hyperlink ref="B17" r:id="rId14"/>
+    <hyperlink ref="B24" r:id="rId13"/>
+    <hyperlink ref="B22" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
@@ -7939,11 +10585,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -8572,11 +11218,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -9205,11 +11851,11 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>

</xml_diff>

<commit_message>
Atualização da apresentação para o SBES 2016
</commit_message>
<xml_diff>
--- a/Avaliação/Performance.xlsx
+++ b/Avaliação/Performance.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17127"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="653"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="653" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dados por Commit" sheetId="1" r:id="rId1"/>
-    <sheet name="Dados por Tamanho" sheetId="2" r:id="rId2"/>
-    <sheet name="Dados por Nr. Arquivos" sheetId="3" r:id="rId3"/>
-    <sheet name="Dados por Nr. Nós" sheetId="4" r:id="rId4"/>
+    <sheet name="Planilha2" sheetId="6" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="5" r:id="rId3"/>
+    <sheet name="Dados por Tamanho" sheetId="2" r:id="rId4"/>
+    <sheet name="Dados por Nr. Arquivos" sheetId="3" r:id="rId5"/>
+    <sheet name="Dados por Nr. Nós" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="85">
   <si>
     <t>Lista de repositórios obtida em https://git.wiki.kernel.org/index.php/GitProjects</t>
   </si>
@@ -240,11 +242,44 @@
   <si>
     <t>Memory Commit History</t>
   </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>0.83</t>
+  </si>
+  <si>
+    <t>-0.05</t>
+  </si>
+  <si>
+    <t>0.88</t>
+  </si>
+  <si>
+    <t>0.96</t>
+  </si>
+  <si>
+    <t>0.76</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.52</t>
+  </si>
+  <si>
+    <t>-0.04</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -351,7 +386,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -382,13 +417,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -401,7 +471,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -445,7 +515,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -598,6 +667,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4E14-480A-A498-6D9F542E1F5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -716,6 +790,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-4E14-480A-A498-6D9F542E1F5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -834,6 +913,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-4E14-480A-A498-6D9F542E1F5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -952,6 +1036,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-4E14-480A-A498-6D9F542E1F5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1061,6 +1150,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-4E14-480A-A498-6D9F542E1F5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1142,43 +1236,14 @@
           <c:yVal>
             <c:numRef>
               <c:f>'Dados por Commit'!$O$4:$O$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>2.7</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0999999999999996</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>18.2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>19.399999999999999</c:v>
-                </c:pt>
-              </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-4E14-480A-A498-6D9F542E1F5E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1238,7 +1303,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1356,7 +1420,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1437,7 +1500,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1505,7 +1567,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1519,7 +1581,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1672,6 +1733,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5C4C-4181-9E2E-4BCC12895D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1790,6 +1856,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5C4C-4181-9E2E-4BCC12895D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1908,6 +1979,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5C4C-4181-9E2E-4BCC12895D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2026,6 +2102,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5C4C-4181-9E2E-4BCC12895D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -2132,6 +2213,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-5C4C-4181-9E2E-4BCC12895D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -2250,6 +2336,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-5C4C-4181-9E2E-4BCC12895D67}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2284,7 +2375,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2377,7 +2467,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2458,7 +2547,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2526,7 +2614,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2692,6 +2780,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B12B-46E2-B38D-31B55E13536B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2810,6 +2903,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B12B-46E2-B38D-31B55E13536B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2928,6 +3026,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B12B-46E2-B38D-31B55E13536B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -3046,6 +3149,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B12B-46E2-B38D-31B55E13536B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -3152,6 +3260,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B12B-46E2-B38D-31B55E13536B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -3270,6 +3383,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B12B-46E2-B38D-31B55E13536B}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3543,7 +3661,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -3709,6 +3827,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-252B-471B-9C90-11BFF25C254C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -3827,6 +3950,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-252B-471B-9C90-11BFF25C254C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -3945,6 +4073,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-252B-471B-9C90-11BFF25C254C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -4063,6 +4196,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-252B-471B-9C90-11BFF25C254C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -4169,6 +4307,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-252B-471B-9C90-11BFF25C254C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -4287,6 +4430,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-252B-471B-9C90-11BFF25C254C}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -7218,8 +7366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="AZ8" sqref="AZ8:BC8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="AY13" sqref="AY13:BB19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7236,23 +7384,7 @@
     <col min="11" max="11" width="7.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="7.28515625" customWidth="1"/>
     <col min="14" max="14" width="8.5703125" customWidth="1"/>
-    <col min="15" max="15" width="8" customWidth="1"/>
-    <col min="16" max="16" width="9" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="8.140625" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="6" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="6.5703125" hidden="1" customWidth="1"/>
-    <col min="20" max="24" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="9" hidden="1" customWidth="1"/>
-    <col min="26" max="29" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="8" hidden="1" customWidth="1"/>
-    <col min="31" max="34" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="8" hidden="1" customWidth="1"/>
-    <col min="36" max="39" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="7.28515625" hidden="1" customWidth="1"/>
-    <col min="41" max="44" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="45" max="45" width="8" hidden="1" customWidth="1"/>
-    <col min="46" max="49" width="8.42578125" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="8.85546875" customWidth="1"/>
+    <col min="15" max="50" width="11.85546875" hidden="1" customWidth="1"/>
     <col min="51" max="51" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="52" max="52" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="5.28515625" bestFit="1" customWidth="1"/>
@@ -9468,8 +9600,7 @@
         <v>0.83030303030303032</v>
       </c>
       <c r="BB14" s="16">
-        <f t="shared" si="28"/>
-        <v>0.55151515151515151</v>
+        <v>0.76</v>
       </c>
       <c r="BC14" s="16">
         <f t="shared" si="28"/>
@@ -9622,8 +9753,7 @@
         <v>0.83030303030303032</v>
       </c>
       <c r="BB15" s="16">
-        <f t="shared" si="45"/>
-        <v>0.55151515151515151</v>
+        <v>0.76</v>
       </c>
       <c r="BC15" s="16">
         <f t="shared" si="45"/>
@@ -9768,19 +9898,16 @@
         <v>41</v>
       </c>
       <c r="AZ16" s="16">
-        <f>AE18</f>
-        <v>7.878787878787874E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="BA16" s="16">
-        <f t="shared" ref="BA16:BC16" si="52">AF18</f>
-        <v>-3.0303030303030276E-2</v>
+        <v>-0.05</v>
       </c>
       <c r="BB16" s="16">
-        <f t="shared" si="52"/>
-        <v>0.34545454545454546</v>
+        <v>0.72</v>
       </c>
       <c r="BC16" s="16">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="BA16:BC16" si="52">AH18</f>
         <v>1.8181818181818188E-2</v>
       </c>
     </row>
@@ -9926,15 +10053,13 @@
         <v>1</v>
       </c>
       <c r="BA17" s="16">
-        <f t="shared" ref="BA17:BC17" si="69">AK18</f>
-        <v>0.87878787878787878</v>
+        <v>0.88</v>
       </c>
       <c r="BB17" s="16">
-        <f t="shared" si="69"/>
-        <v>0.72121212121212119</v>
+        <v>0.52</v>
       </c>
       <c r="BC17" s="16">
-        <f t="shared" si="69"/>
+        <f t="shared" ref="BA17:BC17" si="69">AM18</f>
         <v>-0.16363636363636358</v>
       </c>
     </row>
@@ -10080,15 +10205,13 @@
         <v>1</v>
       </c>
       <c r="BA18" s="16">
-        <f t="shared" ref="BA18:BC18" si="86">AP18</f>
-        <v>0.94285714285714284</v>
+        <v>0.96</v>
       </c>
       <c r="BB18" s="16">
-        <f t="shared" si="86"/>
-        <v>0.5714285714285714</v>
+        <v>-0.04</v>
       </c>
       <c r="BC18" s="16">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="BA18:BC18" si="86">AR18</f>
         <v>-0.60000000000000009</v>
       </c>
     </row>
@@ -10154,8 +10277,7 @@
         <v>0.87878787878787878</v>
       </c>
       <c r="BB19" s="16">
-        <f t="shared" si="87"/>
-        <v>0.72121212121212119</v>
+        <v>0.52</v>
       </c>
       <c r="BC19" s="16">
         <f t="shared" si="87"/>
@@ -10541,6 +10663,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="G4" s="18"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="H6" s="18"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -11172,7 +11423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
@@ -11805,7 +12056,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>

</xml_diff>